<commit_message>
Corrección en base a observaciones realizadas
</commit_message>
<xml_diff>
--- a/CRONOGRAMA/Itinerario.xlsx
+++ b/CRONOGRAMA/Itinerario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\PPP\PPP-NRC24421\CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE794DC-BE4D-49C1-812A-B071A71BFD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C94704-C0E3-4E97-9041-F8F16536C291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1992,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110:B111"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>